<commit_message>
change to python coding style adjust all sheets width
</commit_message>
<xml_diff>
--- a/CrawlerPractice/YouTubeTrending.xlsx
+++ b/CrawlerPractice/YouTubeTrending.xlsx
@@ -4,19 +4,19 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9804" windowWidth="22943"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2018113" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2018114" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2018-11-03" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2018-11-04" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="304">
   <si>
     <t>Title</t>
   </si>
@@ -714,13 +714,28 @@
     <t>這群人TGOP</t>
   </si>
   <si>
+    <t>龍介仙大戰沈玉琳！問不倒ㄟ台南幹話王？【Yahoo TV 琳惟不亂】</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=4VxeGD4qz9Q</t>
+  </si>
+  <si>
+    <t>23 小時前</t>
+  </si>
+  <si>
+    <t>說好的尊重呢? 不能讓哥哥看到的MV幕後花絮! ♥ 滴妹</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=TLP7wZD_kmA</t>
+  </si>
+  <si>
     <t>「烏龜」鄭可強改編超驚豔　《不愛我就拉倒》大圈粉 | 聲林之王</t>
   </si>
   <si>
     <t>www.youtube.com/watch?v=sDNnEVHVP4I</t>
   </si>
   <si>
-    <t>躲喵喵比賽 Yummy媽媽會發現我們嗎？</t>
+    <t>躲喵喵比賽 姐姐跟妹妹誰會先被找到 玩具開箱一起玩玩具Sunny Yummy Kids TOYs</t>
   </si>
   <si>
     <t>www.youtube.com/watch?v=V-5kecMrN0o</t>
@@ -729,7 +744,175 @@
     <t>Sunny&amp;Yummy的玩具箱kids toys</t>
   </si>
   <si>
-    <t>8 小時前</t>
+    <t>韓國瑜嚇到了  陳其邁勞工造勢晚會湧入上萬人,影片0：42～0:53為大寮場人數也暴滿</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=iNx0lcSxvJc</t>
+  </si>
+  <si>
+    <t>ξύλου Δάσος</t>
+  </si>
+  <si>
+    <t>21 小時前</t>
+  </si>
+  <si>
+    <t>嘗試敲爆男友手機！男友怒了竟自摔！？【眾量級CROWD│PRANK互整情侶特輯】</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=Yevw2hTzk9Y</t>
+  </si>
+  <si>
+    <t>韓國瑜見陳樹菊，最強菜販碰頭。</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=60vk4MASFJ4</t>
+  </si>
+  <si>
+    <t>【1104】卡提諾狂新聞 #140</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=r59trF3yMh0</t>
+  </si>
+  <si>
+    <t>10 小時前</t>
+  </si>
+  <si>
+    <t>外星人造訪過地球最有力的證據，納斯卡線 | KUAIZERO</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=tp-_seweHDM</t>
+  </si>
+  <si>
+    <t>상큼 폭발♡ 중독성甲 트둥이들(TWICE)의 히트곡 메들리♬ 아는 형님(Knowing bros) 152회</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=I8evBGAoKcg</t>
+  </si>
+  <si>
+    <t>JTBC Entertainment</t>
+  </si>
+  <si>
+    <t>【博恩夜夜秀】欸！能源難題</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=XUV7ukodLuU</t>
+  </si>
+  <si>
+    <t>STR Network</t>
+  </si>
+  <si>
+    <t>韓國人第一次體驗台灣早餐店, 讓我驚訝的是... ft.Mira's Garden</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=jfWuXSeoYIs</t>
+  </si>
+  <si>
+    <t>京欽 KyeongHeum 경흠</t>
+  </si>
+  <si>
+    <t>劉寶傑被政府施壓？他預言將為韓國瑜催出幾萬票      -     最新消息</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=Lv1s6BY8ewg</t>
+  </si>
+  <si>
+    <t>消息最新</t>
+  </si>
+  <si>
+    <t>13 小時前</t>
+  </si>
+  <si>
+    <t>聲林之王EP4精華｜超炸卑南族語Rap《帥到分手》神remix 潘帥誇林孟辰根本是專業明星｜蕭敬騰 林宥嘉 潘瑋柏</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=YaOYGh3Tzoc</t>
+  </si>
+  <si>
+    <t>聲林之王</t>
+  </si>
+  <si>
+    <t>JJ又一經典！JJ林俊杰中西改編《延禧攻略》《雪落下的聲音》《夢想的聲音3》花絮 EP2 20181102 /浙江衛視官方音樂HD/</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=CPn8SFbAcv4</t>
+  </si>
+  <si>
+    <t>劉寶傑請辭《關鍵時刻》真正原因？朱學恒淚回應</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=q4kxvFjB0H0</t>
+  </si>
+  <si>
+    <t>Mr.Bamboo</t>
+  </si>
+  <si>
+    <t>最新民調韓國瑜領先陳其邁達11%！韓風起逼民進黨選戰亂了套？少康戰情室 20181102</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=eOdtaBgwyug</t>
+  </si>
+  <si>
+    <t>少康戰情室</t>
+  </si>
+  <si>
+    <t>【完整版】主持人真的有斷層嗎？兩代外景主持人比一比2018.11.02小明星大跟班</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=YeozuCThnrw</t>
+  </si>
+  <si>
+    <t>【蔡桃貴】吐奶秀！好大一口啊！</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=MiG6NL1_UwY</t>
+  </si>
+  <si>
+    <t>蔡桃貴</t>
+  </si>
+  <si>
+    <t>可惡想住！羅志祥"家中開車"照片曝光網友歪樓看"鞋櫃" 蕭敬騰豪宅應有盡有游泳池、籃球場超豪華｜【娛樂星世界】20181103｜三立新聞台</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=d5FmkA6mazA</t>
+  </si>
+  <si>
+    <t>54Free食代</t>
+  </si>
+  <si>
+    <t>深入綠票倉!韓國瑜一現身支持者熱情包圍</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=w_9p6HoP_co</t>
+  </si>
+  <si>
+    <t>台視新聞TTV NEWS</t>
+  </si>
+  <si>
+    <t>K/DA - POP/STARS (ft Madison Beer, (G)I-DLE, Jaira Burns) | Official Music Video - League of Legends</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=UOxkGD8qRB4</t>
+  </si>
+  <si>
+    <t>League of Legends</t>
+  </si>
+  <si>
+    <t>Giọng ải giọng ai 3|Tập 14 full: Trường Giang "hả hê" khi tình chị em của Sam - Diệu Nhi "rạn nứt"</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=PmJ0ANzk9qo</t>
+  </si>
+  <si>
+    <t>DIEN QUAN Entertainment / Giải Trí</t>
+  </si>
+  <si>
+    <t>【狠愛演】挑戰一貫3000元,超貴超巨大軍艦壽司『震撼壽司界』</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=MfPZWtZ0TD8</t>
+  </si>
+  <si>
+    <t>狠愛演</t>
   </si>
   <si>
     <t>FULL【蒙面唱将猜猜猜S3】第二期 干净版 歌王超级大揭面 新晋选手神秘登场 20181028 超清1080P</t>
@@ -741,58 +924,185 @@
     <t>蒙面唱將猜猜猜2018第三季华丽归来</t>
   </si>
   <si>
-    <t>可惡想住！羅志祥"家中開車"照片曝光網友歪樓看"鞋櫃" 蕭敬騰豪宅應有盡有游泳池、籃球場超豪華｜【娛樂星世界】20181103｜三立新聞台</t>
-  </si>
-  <si>
-    <t>www.youtube.com/watch?v=d5FmkA6mazA</t>
-  </si>
-  <si>
-    <t>54Free食代</t>
-  </si>
-  <si>
-    <t>10 小時前</t>
-  </si>
-  <si>
-    <t>金家好媳婦 第212集 100% Wife EP212【全】</t>
-  </si>
-  <si>
-    <t>www.youtube.com/watch?v=uwy6aCVGhqE</t>
-  </si>
-  <si>
-    <t>11 小時前</t>
-  </si>
-  <si>
-    <t>【蔡桃貴】吐奶秀！好大一口啊！</t>
-  </si>
-  <si>
-    <t>www.youtube.com/watch?v=MiG6NL1_UwY</t>
-  </si>
-  <si>
-    <t>蔡桃貴</t>
-  </si>
-  <si>
-    <t>13 小時前</t>
-  </si>
-  <si>
-    <t>【狠愛演】挑戰一貫3000元,超貴超巨大軍艦壽司『震撼壽司界』</t>
-  </si>
-  <si>
-    <t>www.youtube.com/watch?v=MfPZWtZ0TD8</t>
-  </si>
-  <si>
-    <t>狠愛演</t>
+    <t>金家好媳婦 第211集 100% Wife EP211【全】</t>
+  </si>
+  <si>
+    <t>www.youtube.com/watch?v=WkPM4i40eh0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="4">
+    <numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" numFmtId="164"/>
+    <numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-" numFmtId="165"/>
+    <numFmt formatCode="_-&quot;NT$&quot;* #,##0_-;\-&quot;NT$&quot;* #,##0_-;_-&quot;NT$&quot;* &quot;-&quot;_-;_-@_-" numFmtId="166"/>
+    <numFmt formatCode="_-&quot;NT$&quot;* #,##0.00_-;\-&quot;NT$&quot;* #,##0.00_-;_-&quot;NT$&quot;* &quot;-&quot;??_-;_-@_-" numFmtId="167"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -800,20 +1110,319 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -824,17 +1433,212 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="49">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="164">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="165">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="166">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="167">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="6" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="15" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="27" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="18" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="9" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="9" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="49">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -1119,7 +1923,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1131,16 +1934,16 @@
   </sheetPr>
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="5"/>
     <col customWidth="1" max="2" min="2" width="100"/>
     <col customWidth="1" max="3" min="3" width="40"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
+    <col customWidth="1" max="5" min="4" width="15"/>
     <col customWidth="1" max="5" min="5" width="15"/>
   </cols>
   <sheetData>
@@ -2672,633 +3475,640 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="5"/>
+    <col customWidth="1" max="2" min="2" width="100"/>
+    <col customWidth="1" max="3" min="3" width="40"/>
+    <col customWidth="1" max="5" min="4" width="15"/>
+    <col customWidth="1" max="5" min="5" width="15"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E2" t="n">
-        <v>437656</v>
+        <v>698136</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>235</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>236</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="E3" t="n">
-        <v>303381</v>
+        <v>586238</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>4645966</v>
+        <v>357294</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>727636</v>
+        <v>5315112</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>428575</v>
+        <v>557562</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
         <v>143</v>
       </c>
       <c r="E7" t="n">
-        <v>432853</v>
+        <v>583092</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>240</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
       <c r="E8" t="n">
-        <v>296441</v>
+        <v>52790</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>244</v>
       </c>
       <c r="E9" t="n">
-        <v>153835</v>
+        <v>204283</v>
       </c>
       <c r="F9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="n">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="n">
+        <v>526490</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E11" t="n">
+        <v>426904</v>
+      </c>
+      <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="n">
-        <v>581457</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C11" t="s">
-        <v>235</v>
-      </c>
-      <c r="D11" t="s">
-        <v>236</v>
-      </c>
-      <c r="E11" t="n">
-        <v>26223</v>
-      </c>
-      <c r="F11" t="s">
-        <v>237</v>
-      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E12" t="n">
-        <v>18501590</v>
+        <v>814847</v>
       </c>
       <c r="F12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="n">
+        <v>180812</v>
+      </c>
+      <c r="F13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" t="n">
-        <v>258057</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E14" t="n">
-        <v>329993</v>
+        <v>365759</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>250</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="E15" t="n">
-        <v>691291</v>
+        <v>454142</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="E16" t="n">
-        <v>531003</v>
+        <v>21864512</v>
       </c>
       <c r="F16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="n">
+        <v>339801</v>
+      </c>
+      <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1556500</v>
-      </c>
-      <c r="F17" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E18" t="n">
-        <v>443186</v>
+        <v>636347</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>255</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>256</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>257</v>
       </c>
       <c r="E19" t="n">
-        <v>272845</v>
+        <v>750704</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>258</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>260</v>
       </c>
       <c r="E20" t="n">
-        <v>401804</v>
+        <v>151535</v>
       </c>
       <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" t="n">
+        <v>322033</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" t="s">
+        <v>263</v>
+      </c>
+      <c r="E22" t="n">
+        <v>76178</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="n">
+        <v>168089</v>
+      </c>
+      <c r="F23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>238</v>
-      </c>
-      <c r="C21" t="s">
-        <v>239</v>
-      </c>
-      <c r="D21" t="s">
-        <v>240</v>
-      </c>
-      <c r="E21" t="n">
-        <v>200158</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1005943</v>
-      </c>
-      <c r="F22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" t="n">
-        <v>488387</v>
-      </c>
-      <c r="F23" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>264</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>266</v>
       </c>
       <c r="E24" t="n">
-        <v>96486</v>
+        <v>126028</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>268</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>269</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>270</v>
       </c>
       <c r="E25" t="n">
-        <v>5410822</v>
+        <v>73247</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="E26" t="n">
-        <v>201592</v>
+        <v>373808</v>
       </c>
       <c r="F26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="n">
+        <v>561559</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2" t="n">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" t="n">
-        <v>278315</v>
-      </c>
-      <c r="F27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>271</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>272</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E28" t="n">
-        <v>639877</v>
+        <v>260419</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E29" t="n">
-        <v>48378</v>
+        <v>871111</v>
       </c>
       <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>273</v>
+      </c>
+      <c r="C30" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" t="s">
+        <v>275</v>
+      </c>
+      <c r="E30" t="n">
+        <v>251070</v>
+      </c>
+      <c r="F30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" t="n">
-        <v>1559911</v>
-      </c>
-      <c r="F30" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="E31" t="n">
-        <v>871754</v>
+        <v>8153447</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -3311,574 +4121,574 @@
         <v>83</v>
       </c>
       <c r="E32" t="n">
-        <v>139576</v>
+        <v>163833</v>
       </c>
       <c r="F32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="n">
+        <v>610952</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="n">
+        <v>363970</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" t="n">
+        <v>717824</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" t="n">
+        <v>726129</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1674791</v>
+      </c>
+      <c r="F37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>276</v>
+      </c>
+      <c r="C38" t="s">
+        <v>277</v>
+      </c>
+      <c r="D38" t="s">
+        <v>278</v>
+      </c>
+      <c r="E38" t="n">
+        <v>312264</v>
+      </c>
+      <c r="F38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" t="n">
-        <v>3064449</v>
-      </c>
-      <c r="F33" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>279</v>
+      </c>
+      <c r="C39" t="s">
+        <v>280</v>
+      </c>
+      <c r="D39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" t="n">
+        <v>176138</v>
+      </c>
+      <c r="F39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" t="s">
-        <v>101</v>
-      </c>
-      <c r="E34" t="n">
-        <v>583693</v>
-      </c>
-      <c r="F34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" t="n">
-        <v>295009</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>241</v>
-      </c>
-      <c r="C36" t="s">
-        <v>242</v>
-      </c>
-      <c r="D36" t="s">
-        <v>243</v>
-      </c>
-      <c r="E36" t="n">
-        <v>59511</v>
-      </c>
-      <c r="F36" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" t="n">
-        <v>463749</v>
-      </c>
-      <c r="F37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" t="n">
-        <v>839768</v>
-      </c>
-      <c r="F38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>245</v>
-      </c>
-      <c r="C39" t="s">
-        <v>246</v>
-      </c>
-      <c r="D39" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" t="n">
-        <v>106598</v>
-      </c>
-      <c r="F39" t="s">
-        <v>247</v>
-      </c>
-    </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>281</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>282</v>
       </c>
       <c r="D40" t="s">
-        <v>110</v>
+        <v>283</v>
       </c>
       <c r="E40" t="n">
-        <v>488955</v>
+        <v>134905</v>
       </c>
       <c r="F40" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="E41" t="n">
-        <v>89267</v>
+        <v>234181</v>
       </c>
       <c r="F41" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>284</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>285</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>286</v>
       </c>
       <c r="E42" t="n">
-        <v>266808</v>
+        <v>85647</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="E43" t="n">
-        <v>112069</v>
+        <v>311412</v>
       </c>
       <c r="F43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>287</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>288</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
+        <v>289</v>
       </c>
       <c r="E44" t="n">
-        <v>1380175</v>
+        <v>127096</v>
       </c>
       <c r="F44" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>248</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>249</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
-        <v>250</v>
+        <v>61</v>
       </c>
       <c r="E45" t="n">
-        <v>100153</v>
+        <v>1057943</v>
       </c>
       <c r="F45" t="s">
-        <v>251</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>290</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>291</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>292</v>
       </c>
       <c r="E46" t="n">
-        <v>167420</v>
+        <v>7821933</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="E47" t="n">
-        <v>282550</v>
+        <v>569500</v>
       </c>
       <c r="F47" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="E48" t="n">
-        <v>379349</v>
+        <v>429972</v>
       </c>
       <c r="F48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" t="n">
+        <v>108958</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>293</v>
+      </c>
+      <c r="C50" t="s">
+        <v>294</v>
+      </c>
+      <c r="D50" t="s">
+        <v>295</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3283222</v>
+      </c>
+      <c r="F50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3505727</v>
+      </c>
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1681975</v>
+      </c>
+      <c r="F52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
         <v>126</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C53" t="s">
         <v>127</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D53" t="s">
         <v>128</v>
       </c>
-      <c r="E49" t="n">
-        <v>16963814</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E53" t="n">
+        <v>18521113</v>
+      </c>
+      <c r="F53" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
-        <v>132</v>
-      </c>
-      <c r="C50" t="s">
-        <v>133</v>
-      </c>
-      <c r="D50" t="s">
-        <v>134</v>
-      </c>
-      <c r="E50" t="n">
-        <v>172251</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1" t="n">
+    <row r="54" spans="1:6">
+      <c r="A54" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" t="n">
+        <v>580257</v>
+      </c>
+      <c r="F54" t="s">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" t="s">
-        <v>137</v>
-      </c>
-      <c r="E51" t="n">
-        <v>273430</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>141</v>
-      </c>
-      <c r="C52" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" t="s">
-        <v>143</v>
-      </c>
-      <c r="E52" t="n">
-        <v>463170</v>
-      </c>
-      <c r="F52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>138</v>
-      </c>
-      <c r="C53" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" t="n">
-        <v>528336</v>
-      </c>
-      <c r="F53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
         <v>159</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>160</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>22</v>
       </c>
-      <c r="E54" t="n">
-        <v>854055</v>
-      </c>
-      <c r="F54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>161</v>
-      </c>
-      <c r="C55" t="s">
-        <v>162</v>
-      </c>
-      <c r="D55" t="s">
-        <v>163</v>
-      </c>
       <c r="E55" t="n">
-        <v>435952</v>
+        <v>872571</v>
       </c>
       <c r="F55" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" t="n">
+        <v>454378</v>
+      </c>
+      <c r="F56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
         <v>164</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>165</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>166</v>
       </c>
-      <c r="E56" t="n">
-        <v>2053655</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E57" t="n">
+        <v>2142986</v>
+      </c>
+      <c r="F57" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="58" spans="1:6">
+      <c r="A58" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
         <v>171</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>172</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>173</v>
       </c>
-      <c r="E57" t="n">
-        <v>359638</v>
-      </c>
-      <c r="F57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>168</v>
-      </c>
-      <c r="C58" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58" t="s">
-        <v>170</v>
-      </c>
       <c r="E58" t="n">
-        <v>507523</v>
+        <v>371505</v>
       </c>
       <c r="F58" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="C59" t="s">
-        <v>175</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="E59" t="n">
-        <v>752746</v>
+        <v>524885</v>
       </c>
       <c r="F59" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="E60" t="n">
-        <v>749476</v>
+        <v>512130</v>
       </c>
       <c r="F60" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="s">
@@ -3891,14 +4701,14 @@
         <v>180</v>
       </c>
       <c r="E61" t="n">
-        <v>1313277</v>
+        <v>1385557</v>
       </c>
       <c r="F61" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>60</v>
       </c>
       <c r="B62" t="s">
@@ -3911,14 +4721,14 @@
         <v>183</v>
       </c>
       <c r="E62" t="n">
-        <v>512956</v>
+        <v>519891</v>
       </c>
       <c r="F62" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>61</v>
       </c>
       <c r="B63" t="s">
@@ -3931,174 +4741,174 @@
         <v>186</v>
       </c>
       <c r="E63" t="n">
-        <v>37909217</v>
+        <v>39080061</v>
       </c>
       <c r="F63" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" t="s">
+        <v>191</v>
+      </c>
+      <c r="D64" t="s">
+        <v>192</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1234049</v>
+      </c>
+      <c r="F64" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E65" t="n">
+        <v>305024</v>
+      </c>
+      <c r="F65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
         <v>187</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>188</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D66" t="s">
         <v>189</v>
       </c>
-      <c r="E64" t="n">
-        <v>471678</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E66" t="n">
+        <v>479284</v>
+      </c>
+      <c r="F66" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>252</v>
-      </c>
-      <c r="C65" t="s">
-        <v>253</v>
-      </c>
-      <c r="D65" t="s">
-        <v>254</v>
-      </c>
-      <c r="E65" t="n">
-        <v>374540</v>
-      </c>
-      <c r="F65" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>190</v>
-      </c>
-      <c r="C66" t="s">
-        <v>191</v>
-      </c>
-      <c r="D66" t="s">
-        <v>192</v>
-      </c>
-      <c r="E66" t="n">
-        <v>1166064</v>
-      </c>
-      <c r="F66" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>296</v>
+      </c>
+      <c r="C67" t="s">
+        <v>297</v>
+      </c>
+      <c r="D67" t="s">
+        <v>298</v>
+      </c>
+      <c r="E67" t="n">
+        <v>382920</v>
+      </c>
+      <c r="F67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
         <v>193</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>194</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>195</v>
       </c>
-      <c r="E67" t="n">
-        <v>779377</v>
-      </c>
-      <c r="F67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>196</v>
-      </c>
-      <c r="C68" t="s">
-        <v>197</v>
-      </c>
-      <c r="D68" t="s">
-        <v>198</v>
-      </c>
       <c r="E68" t="n">
-        <v>355801</v>
+        <v>795316</v>
       </c>
       <c r="F68" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>299</v>
       </c>
       <c r="C69" t="s">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D69" t="s">
-        <v>201</v>
+        <v>301</v>
       </c>
       <c r="E69" t="n">
-        <v>440270</v>
+        <v>229245</v>
       </c>
       <c r="F69" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C70" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D70" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E70" t="n">
-        <v>642955</v>
+        <v>359577</v>
       </c>
       <c r="F70" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C71" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D71" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E71" t="n">
-        <v>943751</v>
+        <v>471440</v>
       </c>
       <c r="F71" t="s">
-        <v>208</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>70</v>
       </c>
       <c r="B72" t="s">
@@ -4111,110 +4921,50 @@
         <v>211</v>
       </c>
       <c r="E72" t="n">
-        <v>177122</v>
+        <v>192712</v>
       </c>
       <c r="F72" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>212</v>
+        <v>302</v>
       </c>
       <c r="C73" t="s">
-        <v>213</v>
+        <v>303</v>
       </c>
       <c r="D73" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E73" t="n">
-        <v>852550</v>
+        <v>237321</v>
       </c>
       <c r="F73" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D74" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="E74" t="n">
-        <v>269884</v>
+        <v>946941</v>
       </c>
       <c r="F74" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>218</v>
-      </c>
-      <c r="C75" t="s">
-        <v>219</v>
-      </c>
-      <c r="D75" t="s">
-        <v>220</v>
-      </c>
-      <c r="E75" t="n">
-        <v>650042</v>
-      </c>
-      <c r="F75" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
-        <v>223</v>
-      </c>
-      <c r="C76" t="s">
-        <v>224</v>
-      </c>
-      <c r="D76" t="s">
-        <v>225</v>
-      </c>
-      <c r="E76" t="n">
-        <v>337085</v>
-      </c>
-      <c r="F76" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="s">
-        <v>226</v>
-      </c>
-      <c r="C77" t="s">
-        <v>227</v>
-      </c>
-      <c r="D77" t="s">
-        <v>228</v>
-      </c>
-      <c r="E77" t="n">
-        <v>707074</v>
-      </c>
-      <c r="F77" t="s">
-        <v>49</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>